<commit_message>
database connecting, but not returning data
</commit_message>
<xml_diff>
--- a/perms.xlsx
+++ b/perms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjcurrie\Documents\GitHub\project0-ers-api-kennethcurrie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{BA2A6844-CDFC-4F81-B85B-52F521E61B8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE807E13-47AF-424A-8A48-12A4CDE3CD66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4485" xr2:uid="{C5D813E6-811A-4EB3-8CD3-5C64778882C9}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Admin</t>
   </si>
@@ -87,7 +87,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,6 +97,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -113,12 +119,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -438,7 +447,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,6 +498,9 @@
       <c r="C3" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F3" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -503,6 +515,9 @@
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F4" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -511,6 +526,9 @@
       <c r="B5" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F5" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -534,6 +552,15 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>